<commit_message>
Update trained model and evaluation
</commit_message>
<xml_diff>
--- a/TrainedModel/0 Helpdesk/1F_A/1F_A_validation.xlsx
+++ b/TrainedModel/0 Helpdesk/1F_A/1F_A_validation.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -385,7 +385,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.8061680469289165</v>
+        <v>0.8191710965728389</v>
       </c>
     </row>
     <row r="3">
@@ -395,7 +395,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.6785196687370602</v>
+        <v>0.6911928379723146</v>
       </c>
     </row>
     <row r="4">
@@ -405,7 +405,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.5453416149068322</v>
+        <v>0.6127929849545581</v>
       </c>
     </row>
     <row r="5">
@@ -415,7 +415,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.811128364389234</v>
+        <v>0.8355975013180249</v>
       </c>
     </row>
     <row r="6">
@@ -425,7 +425,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.5539855072463767</v>
+        <v>0.113646288209607</v>
       </c>
     </row>
     <row r="7">
@@ -435,7 +435,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.8286231884057971</v>
+        <v>0.8693859472243745</v>
       </c>
     </row>
     <row r="8">
@@ -445,7 +445,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.8348837209302326</v>
+        <v>0.8677175529710088</v>
       </c>
     </row>
     <row r="9">
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.9306201550387597</v>
+        <v>0.9281977665618217</v>
       </c>
     </row>
     <row r="10">
@@ -465,7 +465,27 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.4398148148148148</v>
+        <v>0.5681212013925768</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>6_1</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.959599044078598</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>6_2</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.6634808853118711</v>
       </c>
     </row>
   </sheetData>

</xml_diff>